<commit_message>
Feat Insert with wizard data
</commit_message>
<xml_diff>
--- a/files/excel/Branch.xlsx
+++ b/files/excel/Branch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Code</t>
   </si>
@@ -27,18 +27,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A55123</t>
-  </si>
-  <si>
-    <t>SUBA551231</t>
-  </si>
-  <si>
-    <t>MXO723</t>
-  </si>
-  <si>
-    <t>SUBMXO7231</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -51,9 +39,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>POSKO</t>
-  </si>
-  <si>
     <t>HEAD OFFICE</t>
   </si>
   <si>
@@ -163,13 +148,22 @@
   </si>
   <si>
     <t xml:space="preserve">Document Type </t>
+  </si>
+  <si>
+    <t>BRANCH1</t>
+  </si>
+  <si>
+    <t>BRANCH2</t>
+  </si>
+  <si>
+    <t>DKIJK0006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +182,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -253,6 +252,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1217,13 +1217,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
     <col min="4" max="5" width="20" customWidth="1"/>
@@ -1232,7 +1232,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1259,112 +1259,114 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
       </c>
       <c r="O2" t="s">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="R2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
       </c>
+      <c r="D3" s="4">
+        <v>-1</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F3" s="6">
         <v>89422356232</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J3" s="2">
         <v>40524</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
       <c r="L3" s="2">
         <v>12</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="R3" s="2">
         <v>522134</v>
@@ -1391,16 +1393,16 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P4" s="4">
         <v>2</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="R4" s="4">
         <v>512312</v>
@@ -1430,7 +1432,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="R5" s="1">
         <v>452415</v>
@@ -1460,7 +1462,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R6" s="4">
         <v>615231</v>
@@ -1474,49 +1476,55 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>-1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1">
         <v>82648995232</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="5">
+        <v>14530</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5</v>
+      </c>
       <c r="L7" s="5">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P7" s="5">
         <v>1</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="R7" s="5">
         <v>515431</v>
@@ -1543,16 +1551,16 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="P8" s="1">
         <v>2</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R8" s="1">
         <v>612123</v>
@@ -1582,7 +1590,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="R9" s="1">
         <v>565512</v>

</xml_diff>